<commit_message>
Mise à jour des fichiers
</commit_message>
<xml_diff>
--- a/documentation/133_GESTPROJ_BOR_SCH.xlsx
+++ b/documentation/133_GESTPROJ_BOR_SCH.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eduetatfr-my.sharepoint.com/personal/nathan_borgeat_studentfr_ch/Documents/EMF/EMF3/EMF3_Informatique/Modules/Développement/133/Projet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="305" documentId="13_ncr:1_{94F179CE-2B95-4054-BCC1-CDC39A0030AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5915A66F-5D02-40F6-9381-E20E69B3A5BA}"/>
+  <xr:revisionPtr revIDLastSave="470" documentId="13_ncr:1_{94F179CE-2B95-4054-BCC1-CDC39A0030AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{262B59F1-D193-4623-945C-145B6F39C2C7}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planning" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="93">
   <si>
     <t>Planning</t>
   </si>
@@ -305,9 +305,6 @@
     <t>Schéma relationnel</t>
   </si>
   <si>
-    <t>Descentes de code</t>
-  </si>
-  <si>
     <t>Borgeat Nathan / 300231</t>
   </si>
   <si>
@@ -351,13 +348,79 @@
   </si>
   <si>
     <t>Implémentation RestUser</t>
+  </si>
+  <si>
+    <t>Correction Analyse</t>
+  </si>
+  <si>
+    <t>Implémentation RestUser terminée</t>
+  </si>
+  <si>
+    <t>Test du RestUser</t>
+  </si>
+  <si>
+    <t>Diagramme de navigation admin</t>
+  </si>
+  <si>
+    <t>Diagramme de classe admin</t>
+  </si>
+  <si>
+    <t>Elaboration DB admin</t>
+  </si>
+  <si>
+    <t>Implémentation Rest admin</t>
+  </si>
+  <si>
+    <t>Documentation de projet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Problème avec la machine </t>
+  </si>
+  <si>
+    <t>Implémentation de l'API Gateway</t>
+  </si>
+  <si>
+    <t>Test en conteneur du RestUser + API</t>
+  </si>
+  <si>
+    <t>Implémentation contrôleur + services Rest admin</t>
+  </si>
+  <si>
+    <t>Implémentation login + signin + hash</t>
+  </si>
+  <si>
+    <t>Implémentation HTML +CSS Frontend</t>
+  </si>
+  <si>
+    <t>Implémentation Javascript Frontend</t>
+  </si>
+  <si>
+    <t>Implémentation API Gateway Admin</t>
+  </si>
+  <si>
+    <t>Test API Gateway Admin</t>
+  </si>
+  <si>
+    <t>Correction des problèmes + fonctionnement backend</t>
+  </si>
+  <si>
+    <t>Implémentation Frontend (non-abouti)</t>
+  </si>
+  <si>
+    <t>Frontend user + tests</t>
+  </si>
+  <si>
+    <t>Upload + fin des tests (fin des tests)</t>
+  </si>
+  <si>
+    <t>Tests globaux</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -441,6 +504,12 @@
       <name val="Courier New"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -485,7 +554,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -858,11 +927,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="90"/>
@@ -1015,27 +1099,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1063,8 +1126,41 @@
     <xf numFmtId="2" fontId="4" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1081,10 +1177,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1377,82 +1469,82 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P24"/>
+  <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageLayout" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="7.85546875" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="7.81640625" defaultRowHeight="14.5" outlineLevelRow="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" customWidth="1"/>
+    <col min="1" max="1" width="24.453125" customWidth="1"/>
     <col min="2" max="11" width="8" customWidth="1"/>
-    <col min="12" max="17" width="6.5703125" customWidth="1"/>
+    <col min="12" max="17" width="6.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="59" t="s">
+    <row r="1" spans="1:16" ht="31" x14ac:dyDescent="0.7">
+      <c r="A1" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="59"/>
-      <c r="J1" s="59"/>
-      <c r="K1" s="59"/>
-      <c r="L1" s="59"/>
-      <c r="M1" s="59"/>
-      <c r="N1" s="59"/>
-      <c r="O1" s="59"/>
-      <c r="P1" s="59"/>
-    </row>
-    <row r="2" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:16" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="73"/>
+      <c r="J1" s="73"/>
+      <c r="K1" s="73"/>
+      <c r="L1" s="73"/>
+      <c r="M1" s="73"/>
+      <c r="N1" s="73"/>
+      <c r="O1" s="73"/>
+      <c r="P1" s="73"/>
+    </row>
+    <row r="2" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="1:16" ht="21.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="60" t="s">
+      <c r="B3" s="74" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="62"/>
-      <c r="D3" s="62"/>
-      <c r="E3" s="62"/>
-      <c r="F3" s="62"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="62"/>
-      <c r="I3" s="62"/>
-      <c r="J3" s="62"/>
-      <c r="K3" s="61"/>
+      <c r="C3" s="76"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="76"/>
+      <c r="G3" s="76"/>
+      <c r="H3" s="76"/>
+      <c r="I3" s="76"/>
+      <c r="J3" s="76"/>
+      <c r="K3" s="75"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="N3" s="2"/>
-      <c r="O3" s="60">
+      <c r="O3" s="74">
         <v>300231</v>
       </c>
-      <c r="P3" s="61"/>
-    </row>
-    <row r="4" spans="1:16" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="P3" s="75"/>
+    </row>
+    <row r="4" spans="1:16" ht="21.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="60" t="s">
+      <c r="B4" s="74" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="62"/>
-      <c r="D4" s="62"/>
-      <c r="E4" s="62"/>
-      <c r="F4" s="62"/>
-      <c r="G4" s="62"/>
-      <c r="H4" s="62"/>
-      <c r="I4" s="62"/>
-      <c r="J4" s="62"/>
-      <c r="K4" s="61"/>
+      <c r="C4" s="76"/>
+      <c r="D4" s="76"/>
+      <c r="E4" s="76"/>
+      <c r="F4" s="76"/>
+      <c r="G4" s="76"/>
+      <c r="H4" s="76"/>
+      <c r="I4" s="76"/>
+      <c r="J4" s="76"/>
+      <c r="K4" s="75"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2" t="s">
         <v>3</v>
@@ -1462,35 +1554,35 @@
         <v>133</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="56" t="s">
+    <row r="6" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="7" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B7" s="70" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="57"/>
-      <c r="D7" s="58"/>
-      <c r="E7" s="56" t="s">
+      <c r="C7" s="71"/>
+      <c r="D7" s="72"/>
+      <c r="E7" s="70" t="s">
         <v>25</v>
       </c>
-      <c r="F7" s="57"/>
-      <c r="G7" s="58"/>
-      <c r="H7" s="56" t="s">
+      <c r="F7" s="71"/>
+      <c r="G7" s="72"/>
+      <c r="H7" s="70" t="s">
         <v>26</v>
       </c>
-      <c r="I7" s="57"/>
-      <c r="J7" s="58"/>
-      <c r="K7" s="56" t="s">
+      <c r="I7" s="71"/>
+      <c r="J7" s="72"/>
+      <c r="K7" s="70" t="s">
         <v>27</v>
       </c>
-      <c r="L7" s="57"/>
-      <c r="M7" s="58"/>
-      <c r="N7" s="56" t="s">
+      <c r="L7" s="71"/>
+      <c r="M7" s="72"/>
+      <c r="N7" s="70" t="s">
         <v>28</v>
       </c>
-      <c r="O7" s="57"/>
-      <c r="P7" s="58"/>
-    </row>
-    <row r="8" spans="1:16" s="1" customFormat="1" ht="96" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O7" s="71"/>
+      <c r="P7" s="72"/>
+    </row>
+    <row r="8" spans="1:16" s="1" customFormat="1" ht="96" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="30" t="s">
         <v>4</v>
       </c>
@@ -1540,7 +1632,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="31" t="s">
         <v>20</v>
       </c>
@@ -1570,7 +1662,7 @@
       <c r="O9" s="19"/>
       <c r="P9" s="20"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" s="31" t="s">
         <v>5</v>
       </c>
@@ -1590,7 +1682,7 @@
       <c r="O10" s="41"/>
       <c r="P10" s="43"/>
     </row>
-    <row r="11" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A11" s="32" t="s">
         <v>48</v>
       </c>
@@ -1612,7 +1704,7 @@
       <c r="O11" s="19"/>
       <c r="P11" s="20"/>
     </row>
-    <row r="12" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A12" s="32" t="s">
         <v>49</v>
       </c>
@@ -1634,7 +1726,7 @@
       <c r="O12" s="19"/>
       <c r="P12" s="20"/>
     </row>
-    <row r="13" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A13" s="32" t="s">
         <v>50</v>
       </c>
@@ -1646,7 +1738,9 @@
         <v>33</v>
       </c>
       <c r="G13" s="35"/>
-      <c r="H13" s="38"/>
+      <c r="H13" s="38" t="s">
+        <v>33</v>
+      </c>
       <c r="I13" s="19"/>
       <c r="J13" s="20"/>
       <c r="K13" s="22"/>
@@ -1656,7 +1750,7 @@
       <c r="O13" s="19"/>
       <c r="P13" s="20"/>
     </row>
-    <row r="14" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A14" s="32" t="s">
         <v>51</v>
       </c>
@@ -1678,7 +1772,7 @@
       <c r="O14" s="19"/>
       <c r="P14" s="20"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" s="31" t="s">
         <v>6</v>
       </c>
@@ -1698,7 +1792,7 @@
       <c r="O15" s="41"/>
       <c r="P15" s="43"/>
     </row>
-    <row r="16" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A16" s="32" t="s">
         <v>52</v>
       </c>
@@ -1708,8 +1802,12 @@
       <c r="E16" s="22"/>
       <c r="F16" s="19"/>
       <c r="G16" s="20"/>
-      <c r="H16" s="36"/>
-      <c r="I16" s="17"/>
+      <c r="H16" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="I16" s="17" t="s">
+        <v>33</v>
+      </c>
       <c r="J16" s="20"/>
       <c r="K16" s="22"/>
       <c r="L16" s="19"/>
@@ -1718,7 +1816,7 @@
       <c r="O16" s="19"/>
       <c r="P16" s="20"/>
     </row>
-    <row r="17" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A17" s="32" t="s">
         <v>53</v>
       </c>
@@ -1729,7 +1827,9 @@
       <c r="F17" s="19"/>
       <c r="G17" s="20"/>
       <c r="H17" s="36"/>
-      <c r="I17" s="17"/>
+      <c r="I17" s="17" t="s">
+        <v>33</v>
+      </c>
       <c r="J17" s="20"/>
       <c r="K17" s="22"/>
       <c r="L17" s="19"/>
@@ -1738,7 +1838,7 @@
       <c r="O17" s="19"/>
       <c r="P17" s="20"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" collapsed="1" x14ac:dyDescent="0.35">
       <c r="A18" s="32" t="s">
         <v>54</v>
       </c>
@@ -1747,7 +1847,9 @@
       <c r="D18" s="23"/>
       <c r="E18" s="22"/>
       <c r="F18" s="19"/>
-      <c r="G18" s="20"/>
+      <c r="G18" s="20" t="s">
+        <v>33</v>
+      </c>
       <c r="H18" s="38"/>
       <c r="I18" s="17"/>
       <c r="J18" s="20"/>
@@ -1758,7 +1860,7 @@
       <c r="O18" s="19"/>
       <c r="P18" s="20"/>
     </row>
-    <row r="19" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A19" s="32" t="s">
         <v>55</v>
       </c>
@@ -1768,7 +1870,9 @@
       <c r="E19" s="22"/>
       <c r="F19" s="19"/>
       <c r="G19" s="20"/>
-      <c r="H19" s="38"/>
+      <c r="H19" s="38" t="s">
+        <v>33</v>
+      </c>
       <c r="I19" s="17"/>
       <c r="J19" s="20"/>
       <c r="K19" s="22"/>
@@ -1778,7 +1882,7 @@
       <c r="O19" s="19"/>
       <c r="P19" s="20"/>
     </row>
-    <row r="20" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A20" s="31" t="s">
         <v>7</v>
       </c>
@@ -1789,18 +1893,34 @@
       <c r="F20" s="39"/>
       <c r="G20" s="47"/>
       <c r="H20" s="38"/>
-      <c r="I20" s="39"/>
-      <c r="J20" s="35"/>
-      <c r="K20" s="16"/>
-      <c r="L20" s="17"/>
-      <c r="M20" s="35"/>
-      <c r="N20" s="45"/>
-      <c r="O20" s="39"/>
-      <c r="P20" s="47"/>
-    </row>
-    <row r="21" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="32" t="s">
-        <v>56</v>
+      <c r="I20" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="J20" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="K20" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="L20" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="M20" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="N20" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="O20" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="P20" s="47" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="31" t="s">
+        <v>8</v>
       </c>
       <c r="B21" s="22"/>
       <c r="C21" s="19"/>
@@ -1811,76 +1931,78 @@
       <c r="H21" s="21"/>
       <c r="I21" s="19"/>
       <c r="J21" s="20"/>
-      <c r="K21" s="22"/>
+      <c r="K21" s="22" t="s">
+        <v>33</v>
+      </c>
       <c r="L21" s="19"/>
-      <c r="M21" s="20"/>
-      <c r="N21" s="22"/>
-      <c r="O21" s="19"/>
-      <c r="P21" s="20"/>
-    </row>
-    <row r="22" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="B22" s="22"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="23"/>
+      <c r="M21" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="N21" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="O21" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="P21" s="20" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A22" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="24"/>
+      <c r="C22" s="25"/>
+      <c r="D22" s="48"/>
       <c r="E22" s="22"/>
       <c r="F22" s="19"/>
       <c r="G22" s="20"/>
-      <c r="H22" s="21"/>
-      <c r="I22" s="19"/>
-      <c r="J22" s="20"/>
-      <c r="K22" s="22"/>
-      <c r="L22" s="19"/>
-      <c r="M22" s="20"/>
-      <c r="N22" s="16"/>
-      <c r="O22" s="17"/>
-      <c r="P22" s="20"/>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="B23" s="24"/>
-      <c r="C23" s="25"/>
-      <c r="D23" s="48"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="27"/>
-      <c r="I23" s="25"/>
-      <c r="J23" s="26"/>
-      <c r="K23" s="24"/>
-      <c r="L23" s="25"/>
-      <c r="M23" s="26"/>
-      <c r="N23" s="24"/>
-      <c r="O23" s="49"/>
-      <c r="P23" s="50"/>
-    </row>
-    <row r="24" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="34" t="s">
+      <c r="H22" s="27"/>
+      <c r="I22" s="25"/>
+      <c r="J22" s="26"/>
+      <c r="K22" s="24"/>
+      <c r="L22" s="25"/>
+      <c r="M22" s="26"/>
+      <c r="N22" s="24"/>
+      <c r="O22" s="49"/>
+      <c r="P22" s="50" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="51"/>
-      <c r="C24" s="52"/>
-      <c r="D24" s="53"/>
-      <c r="E24" s="51"/>
-      <c r="F24" s="54" t="s">
-        <v>33</v>
-      </c>
-      <c r="G24" s="55" t="s">
-        <v>33</v>
-      </c>
-      <c r="H24" s="51"/>
-      <c r="I24" s="54"/>
-      <c r="J24" s="55"/>
-      <c r="K24" s="51"/>
-      <c r="L24" s="54"/>
-      <c r="M24" s="55"/>
-      <c r="N24" s="51"/>
-      <c r="O24" s="54"/>
-      <c r="P24" s="55"/>
+      <c r="B23" s="51"/>
+      <c r="C23" s="52"/>
+      <c r="D23" s="53"/>
+      <c r="E23" s="51"/>
+      <c r="F23" s="54" t="s">
+        <v>33</v>
+      </c>
+      <c r="G23" s="55" t="s">
+        <v>33</v>
+      </c>
+      <c r="H23" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="I23" s="54" t="s">
+        <v>33</v>
+      </c>
+      <c r="J23" s="55" t="s">
+        <v>33</v>
+      </c>
+      <c r="K23" s="51"/>
+      <c r="L23" s="54"/>
+      <c r="M23" s="55"/>
+      <c r="N23" s="51"/>
+      <c r="O23" s="54" t="s">
+        <v>33</v>
+      </c>
+      <c r="P23" s="55" t="s">
+        <v>33</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -1910,44 +2032,44 @@
   </sheetPr>
   <dimension ref="A1:C47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView showGridLines="0" view="pageLayout" topLeftCell="A21" zoomScale="85" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" customWidth="1"/>
-    <col min="2" max="2" width="63.85546875" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.453125" customWidth="1"/>
+    <col min="2" max="2" width="63.81640625" customWidth="1"/>
+    <col min="3" max="3" width="25.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="59" t="s">
+    <row r="1" spans="1:3" ht="31" x14ac:dyDescent="0.7">
+      <c r="A1" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+    </row>
+    <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="1:3" ht="21.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:3" ht="21.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="7" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
         <v>10</v>
       </c>
@@ -1958,51 +2080,51 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="66">
+    <row r="8" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="59">
         <v>45740</v>
       </c>
-      <c r="B8" s="67" t="s">
-        <v>65</v>
-      </c>
-      <c r="C8" s="68">
+      <c r="B8" s="60" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" s="61">
         <v>1.5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="69">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="62">
         <v>45741</v>
       </c>
-      <c r="B9" s="70" t="s">
-        <v>62</v>
-      </c>
-      <c r="C9" s="71">
+      <c r="B9" s="63" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" s="64">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="11">
         <v>45741</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C10" s="12">
         <v>0.5</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="11">
         <v>45741</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C11" s="12">
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="11">
         <v>45741</v>
       </c>
@@ -2013,211 +2135,279 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="66">
+    <row r="13" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="59">
         <v>45741</v>
       </c>
-      <c r="B13" s="67" t="s">
+      <c r="B13" s="60" t="s">
         <v>54</v>
       </c>
-      <c r="C13" s="68">
+      <c r="C13" s="61">
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="63">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" s="62">
         <v>45747</v>
       </c>
-      <c r="B14" s="64" t="s">
+      <c r="B14" s="63" t="s">
         <v>50</v>
       </c>
-      <c r="C14" s="65">
+      <c r="C14" s="64">
         <v>0.5</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="11">
         <v>45747</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C15" s="12">
         <v>0.25</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="11">
         <v>45747</v>
       </c>
-      <c r="B16" s="72" t="s">
+      <c r="B16" s="65" t="s">
         <v>22</v>
       </c>
       <c r="C16" s="12">
         <v>1.25</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="11">
         <v>45747</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C17" s="12">
         <v>2.5</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="11">
         <v>45747</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="65" t="s">
         <v>71</v>
       </c>
-      <c r="C18" s="12"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="12"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="11"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="12"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="11"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="12"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="11"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="12"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="11"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="12"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="11"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="12"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="11"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="12"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="11"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="12"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="11"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="12"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="11"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="12"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="11"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="12"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C18" s="12">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="59">
+        <v>45747</v>
+      </c>
+      <c r="B19" s="60" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" s="61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" s="62">
+        <v>45748</v>
+      </c>
+      <c r="B20" s="63" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" s="64">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="59">
+        <v>45748</v>
+      </c>
+      <c r="B21" s="60" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" s="61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" s="56">
+        <v>45754</v>
+      </c>
+      <c r="B22" s="57" t="s">
+        <v>79</v>
+      </c>
+      <c r="C22" s="58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" s="11">
+        <v>45754</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C23" s="12">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="59">
+        <v>45754</v>
+      </c>
+      <c r="B24" s="60" t="s">
+        <v>81</v>
+      </c>
+      <c r="C24" s="61">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="66">
+        <v>45755</v>
+      </c>
+      <c r="B25" s="67" t="s">
+        <v>88</v>
+      </c>
+      <c r="C25" s="68">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="66">
+        <v>45761</v>
+      </c>
+      <c r="B26" s="69" t="s">
+        <v>90</v>
+      </c>
+      <c r="C26" s="68">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" s="56">
+        <v>45762</v>
+      </c>
+      <c r="B27" s="57" t="s">
+        <v>91</v>
+      </c>
+      <c r="C27" s="58">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" s="11">
+        <v>45762</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C28" s="12">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" s="11">
+        <v>45762</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29" s="12">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="11"/>
       <c r="B30" s="8"/>
       <c r="C30" s="12"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="11"/>
       <c r="B31" s="8"/>
       <c r="C31" s="12"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="11"/>
       <c r="B32" s="8"/>
       <c r="C32" s="12"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="11"/>
       <c r="B33" s="8"/>
       <c r="C33" s="12"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="11"/>
       <c r="B34" s="8"/>
       <c r="C34" s="12"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="11"/>
       <c r="B35" s="8"/>
       <c r="C35" s="12"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="11"/>
       <c r="B36" s="8"/>
       <c r="C36" s="12"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="11"/>
       <c r="B37" s="8"/>
       <c r="C37" s="12"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="11"/>
       <c r="B38" s="8"/>
       <c r="C38" s="12"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="11"/>
       <c r="B39" s="8"/>
       <c r="C39" s="12"/>
     </row>
-    <row r="40" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A40" s="9" t="s">
         <v>13</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="12">
         <f>SUM(C8:C39)</f>
-        <v>9.5</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+        <v>36.5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B42" s="13" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B43" s="14" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B44" s="15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B45" s="14" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B46" s="15" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B47" s="15" t="s">
         <v>19</v>
       </c>
@@ -2227,7 +2417,7 @@
     <mergeCell ref="A1:C1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="80" fitToHeight="0" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="80" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;LModule 133&amp;RJournal de travail</oddHeader>
     <oddFooter>&amp;C&amp;D&amp;R&amp;P/&amp;N</oddFooter>
@@ -2240,48 +2430,48 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageLayout" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView showGridLines="0" view="pageLayout" topLeftCell="A30" zoomScale="115" zoomScaleNormal="100" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" customWidth="1"/>
-    <col min="2" max="2" width="63.85546875" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.453125" customWidth="1"/>
+    <col min="2" max="2" width="63.81640625" customWidth="1"/>
+    <col min="3" max="3" width="25.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="59" t="s">
+    <row r="1" spans="1:3" ht="31" x14ac:dyDescent="0.7">
+      <c r="A1" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+    </row>
+    <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="1:3" ht="21.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="21.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="7" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
         <v>10</v>
       </c>
@@ -2292,137 +2482,274 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="11">
         <v>45740</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C8" s="12">
         <v>1.5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="11">
         <v>45741</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C9" s="12">
         <v>1.5</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="11">
         <v>45741</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C10" s="12">
         <v>0.5</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="11">
         <v>45741</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C11" s="12">
         <v>1.5</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="12"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="12"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="11"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="12"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="11"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="12"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="12"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="11"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="12"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="11"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="12"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="12"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="11"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="12"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="11"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="12"/>
-    </row>
-    <row r="22" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" s="11">
+        <v>45747</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C12" s="12">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" s="11">
+        <v>45747</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C13" s="12">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" s="11">
+        <v>45747</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C14" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" s="11">
+        <v>45748</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C15" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" s="11">
+        <v>45748</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C16" s="12">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" s="11">
+        <v>45754</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C17" s="12">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" s="11">
+        <v>45754</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C18" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" s="11">
+        <v>45754</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C19" s="12">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" s="11">
+        <v>45754</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C20" s="12">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" s="11">
+        <v>45754</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C21" s="12">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" s="11">
+        <v>45755</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C22" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" s="11">
+        <v>45755</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C23" s="12">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" s="11">
+        <v>45761</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C24" s="12">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" s="11">
+        <v>45761</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C25" s="12">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" s="11">
+        <v>45762</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="C26" s="12">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" s="11">
+        <v>45762</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" s="12">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" s="11">
+        <v>45762</v>
+      </c>
+      <c r="B28" s="65" t="s">
+        <v>78</v>
+      </c>
+      <c r="C28" s="12">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A29" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B22" s="8"/>
-      <c r="C22" s="12">
-        <f>SUM(C8:C21)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="13" t="s">
+      <c r="B29" s="8"/>
+      <c r="C29" s="12">
+        <f>SUM(C8:C28)</f>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B31" s="13" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B25" s="14" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B32" s="14" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B26" s="15" t="s">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B33" s="15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B27" s="14" t="s">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B34" s="14" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B28" s="15" t="s">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B35" s="15" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B29" s="15" t="s">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B36" s="15" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2431,7 +2758,7 @@
     <mergeCell ref="A1:C1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="80" fitToHeight="0" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="80" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;LModule 133&amp;RJournal de travail</oddHeader>
     <oddFooter>&amp;C&amp;D&amp;R&amp;P/&amp;N</oddFooter>
@@ -2440,6 +2767,71 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Self_Registration_Enabled xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <Student_Groups xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Student_Groups>
+    <Distribution_Groups xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <AppVersion xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <Invited_Teachers xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <Templates xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <Has_Teacher_Only_SectionGroup xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <CultureName xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <LMS_Mappings xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <Invited_Students xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <FolderType xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <Teachers xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Teachers>
+    <TeamsChannelId xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <IsNotebookLocked xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <Is_Collaboration_Space_Locked xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <Teams_Channel_Section_Location xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <Math_Settings xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <Owner xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Owner>
+    <Students xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Students>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="3fb344db-9a83-4925-8457-d4a81a8233b7" xsi:nil="true"/>
+    <NotebookType xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+    <DefaultSectionNames xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004EEFC8B7315DA4449F69FE97A704FE57" ma:contentTypeVersion="35" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="c91a1a7a62e987314df808fa39da4b34">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cc3645a1-58b5-4da5-acb4-f681c13b5e81" xmlns:ns3="3fb344db-9a83-4925-8457-d4a81a8233b7" xmlns:ns4="52c6fd7a-766c-4f84-9f35-2a37be325271" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5e3023738844047246cab05fc3830165" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="cc3645a1-58b5-4da5-acb4-f681c13b5e81"/>
@@ -2893,72 +3285,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Self_Registration_Enabled xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <Student_Groups xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Student_Groups>
-    <Distribution_Groups xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <AppVersion xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <Invited_Teachers xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <Templates xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <Has_Teacher_Only_SectionGroup xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <CultureName xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <LMS_Mappings xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <Invited_Students xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <FolderType xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <Teachers xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Teachers>
-    <TeamsChannelId xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <IsNotebookLocked xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <Is_Collaboration_Space_Locked xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <Teams_Channel_Section_Location xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <Math_Settings xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <Owner xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Owner>
-    <Students xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Students>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="3fb344db-9a83-4925-8457-d4a81a8233b7" xsi:nil="true"/>
-    <NotebookType xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-    <DefaultSectionNames xmlns="52c6fd7a-766c-4f84-9f35-2a37be325271" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE473839-D414-4B78-82BC-08E64CD93726}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE303A41-7D70-49B7-87A8-C6207A042BC3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="52c6fd7a-766c-4f84-9f35-2a37be325271"/>
+    <ds:schemaRef ds:uri="3fb344db-9a83-4925-8457-d4a81a8233b7"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{05539879-8A52-4B74-9FF2-F471F780BCE4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2976,23 +3322,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE303A41-7D70-49B7-87A8-C6207A042BC3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="52c6fd7a-766c-4f84-9f35-2a37be325271"/>
-    <ds:schemaRef ds:uri="3fb344db-9a83-4925-8457-d4a81a8233b7"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE473839-D414-4B78-82BC-08E64CD93726}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>